<commit_message>
Login  ACME System 1
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Biti9\Documents\UiPath\ACME_System_ReFrameWork\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C13A71F-D1AE-4A0B-AAEB-A6FDBA2A6EA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B5E203-8616-4E5C-9198-7112418604C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3831" yWindow="1337" windowWidth="16449" windowHeight="9549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,12 +109,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>System1_URL</t>
-  </si>
-  <si>
-    <t>http://www.acme-test.com</t>
-  </si>
-  <si>
     <t>System1 URL</t>
   </si>
   <si>
@@ -131,6 +125,12 @@
   </si>
   <si>
     <t>SHA-1 Onlien URL</t>
+  </si>
+  <si>
+    <t>http://www.acme-test.com/</t>
+  </si>
+  <si>
+    <t>System1_URL</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1"/>
@@ -575,35 +575,35 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1600,9 +1600,10 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{C809F24F-D952-4858-9BF3-813DA789C3C1}"/>
+    <hyperlink ref="B6" r:id="rId2" xr:uid="{2DB15253-E41F-4AC7-881B-E6B8976A5990}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1610,7 +1611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3828125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1660,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>